<commit_message>
menyelesaikan program kankerParuParu dan menambahkan file excel perhitungan
</commit_message>
<xml_diff>
--- a/Data/dataPercobaan.xlsx
+++ b/Data/dataPercobaan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95499214ec9b6c66/Documents/TUGAS ONGOING/SMS 4/PRAK SCPK/ProjectAkhir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95499214ec9b6c66/Documents/TUGAS ONGOING/SMS 4/PRAK SCPK/ProjectAkhir/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="8_{6257C2E4-72F0-4E11-B491-2DEF1B678F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA1F1043-F134-4DBB-B09C-6101BC7DF3B2}"/>
@@ -142,6 +142,10 @@
 </file>
 
 <file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 

</xml_diff>